<commit_message>
Adding .idea to gitignore and updated database
</commit_message>
<xml_diff>
--- a/books/art_database.xlsx
+++ b/books/art_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\PycharmProjects\pythonProject\books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E57BA19-36ED-41BA-8C7D-DBB71BE0FDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BECD235-C4E9-45E9-9DA5-577E118AA44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{53D4F322-FC8F-4374-991E-81A179F8E64B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53D4F322-FC8F-4374-991E-81A179F8E64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="206">
   <si>
     <t>Impresionismo</t>
   </si>
@@ -555,9 +555,6 @@
     <t>Robert Morris</t>
   </si>
   <si>
-    <t>Christo and Jeanne-Claude</t>
-  </si>
-  <si>
     <t>James Turrell</t>
   </si>
   <si>
@@ -649,6 +646,12 @@
   </si>
   <si>
     <t>Año muerte</t>
+  </si>
+  <si>
+    <t>Christo Vladimirov Javacheff</t>
+  </si>
+  <si>
+    <t>Jeanne-Claude Denat de Guillebon</t>
   </si>
 </sst>
 </file>
@@ -1000,32 +1003,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26793DDB-8B93-4CF5-8108-4EF59218E60C}">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" t="s">
         <v>201</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>203</v>
-      </c>
-      <c r="D1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2715,6 +2718,12 @@
       <c r="B122" t="s">
         <v>125</v>
       </c>
+      <c r="C122">
+        <v>1899</v>
+      </c>
+      <c r="D122">
+        <v>1968</v>
+      </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -2723,6 +2732,9 @@
       <c r="B123" t="s">
         <v>126</v>
       </c>
+      <c r="C123">
+        <v>1963</v>
+      </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
@@ -2731,6 +2743,12 @@
       <c r="B124" t="s">
         <v>127</v>
       </c>
+      <c r="C124">
+        <v>1928</v>
+      </c>
+      <c r="D124">
+        <v>2011</v>
+      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -2739,6 +2757,12 @@
       <c r="B125" t="s">
         <v>128</v>
       </c>
+      <c r="C125">
+        <v>1888</v>
+      </c>
+      <c r="D125">
+        <v>1976</v>
+      </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -2747,6 +2771,9 @@
       <c r="B126" t="s">
         <v>130</v>
       </c>
+      <c r="C126">
+        <v>1930</v>
+      </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
@@ -2755,6 +2782,12 @@
       <c r="B127" t="s">
         <v>131</v>
       </c>
+      <c r="C127">
+        <v>1925</v>
+      </c>
+      <c r="D127">
+        <v>2008</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
@@ -2763,525 +2796,827 @@
       <c r="B128" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>129</v>
       </c>
       <c r="B129" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
       <c r="B130" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>129</v>
       </c>
       <c r="B131" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131">
+        <v>1928</v>
+      </c>
+      <c r="D131">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>129</v>
       </c>
       <c r="B132" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C132">
+        <v>1931</v>
+      </c>
+      <c r="D132">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>129</v>
       </c>
       <c r="B133" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>129</v>
       </c>
       <c r="B134" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134">
+        <v>1933</v>
+      </c>
+      <c r="D134">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>129</v>
       </c>
       <c r="B135" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C135">
+        <v>1901</v>
+      </c>
+      <c r="D135">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>129</v>
       </c>
       <c r="B136" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C136">
+        <v>1923</v>
+      </c>
+      <c r="D136">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>129</v>
       </c>
       <c r="B137" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C137">
+        <v>1941</v>
+      </c>
+      <c r="D137">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>129</v>
       </c>
       <c r="B138" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C138">
+        <v>1924</v>
+      </c>
+      <c r="D138">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>129</v>
       </c>
       <c r="B139" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C139">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>129</v>
       </c>
       <c r="B140" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C140">
+        <v>1922</v>
+      </c>
+      <c r="D140">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>129</v>
       </c>
       <c r="B141" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C141">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>129</v>
       </c>
       <c r="B142" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C142">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>129</v>
       </c>
       <c r="B143" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C143">
+        <v>1909</v>
+      </c>
+      <c r="D143">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>129</v>
       </c>
       <c r="B144" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C144">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>129</v>
       </c>
       <c r="B145" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C145">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>129</v>
       </c>
       <c r="B146" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C146">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>129</v>
       </c>
       <c r="B147" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C147">
+        <v>1911</v>
+      </c>
+      <c r="D147">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>129</v>
       </c>
       <c r="B148" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C148">
+        <v>1930</v>
+      </c>
+      <c r="D148">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>153</v>
       </c>
       <c r="B149" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C149">
+        <v>1933</v>
+      </c>
+      <c r="D149">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>153</v>
       </c>
       <c r="B150" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C150">
+        <v>1928</v>
+      </c>
+      <c r="D150">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>153</v>
       </c>
       <c r="B151" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C151">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>153</v>
       </c>
       <c r="B152" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C152">
+        <v>1936</v>
+      </c>
+      <c r="D152">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>153</v>
       </c>
       <c r="B153" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C153">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
       <c r="B154" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C154">
+        <v>1928</v>
+      </c>
+      <c r="D154">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>153</v>
       </c>
       <c r="B155" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C155">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>153</v>
       </c>
       <c r="B156" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C156">
+        <v>1921</v>
+      </c>
+      <c r="D156">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>153</v>
       </c>
       <c r="B157" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C157">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>163</v>
       </c>
       <c r="B158" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C158">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>163</v>
       </c>
       <c r="B159" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C159">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>163</v>
       </c>
       <c r="B160" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C160">
+        <v>1938</v>
+      </c>
+      <c r="D160">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>163</v>
       </c>
       <c r="B161" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C161">
+        <v>1940</v>
+      </c>
+      <c r="D161">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>163</v>
       </c>
       <c r="B162" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C162">
+        <v>1924</v>
+      </c>
+      <c r="D162">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>163</v>
       </c>
       <c r="B163" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C163">
+        <v>1933</v>
+      </c>
+      <c r="D163">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
       <c r="B164" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C164">
+        <v>1932</v>
+      </c>
+      <c r="D164">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>163</v>
       </c>
       <c r="B165" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C165">
+        <v>1943</v>
+      </c>
+      <c r="D165">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>163</v>
       </c>
       <c r="B166" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C166">
+        <v>1931</v>
+      </c>
+      <c r="D166">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>163</v>
       </c>
       <c r="B167" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="C167">
+        <v>1935</v>
+      </c>
+      <c r="D167">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>163</v>
       </c>
       <c r="B168" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="C168">
+        <v>1935</v>
+      </c>
+      <c r="D168">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>163</v>
       </c>
       <c r="B169" t="s">
+        <v>173</v>
+      </c>
+      <c r="C169">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>163</v>
+      </c>
+      <c r="B170" t="s">
+        <v>174</v>
+      </c>
+      <c r="C170">
+        <v>1935</v>
+      </c>
+      <c r="D170">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="B171" t="s">
         <v>176</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C171">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>175</v>
+      </c>
+      <c r="B172" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>176</v>
-      </c>
-      <c r="B171" t="s">
+      <c r="C172">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>175</v>
+      </c>
+      <c r="B173" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>176</v>
-      </c>
-      <c r="B172" t="s">
+      <c r="C173">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>175</v>
+      </c>
+      <c r="B174" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>176</v>
-      </c>
-      <c r="B173" t="s">
+      <c r="C174">
+        <v>1960</v>
+      </c>
+      <c r="D174">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>175</v>
+      </c>
+      <c r="B175" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>176</v>
-      </c>
-      <c r="B174" t="s">
+      <c r="C175">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>176</v>
-      </c>
-      <c r="B175" t="s">
+      <c r="C176">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>175</v>
+      </c>
+      <c r="B177" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>176</v>
-      </c>
-      <c r="B176" t="s">
+      <c r="C177">
+        <v>1958</v>
+      </c>
+      <c r="D177">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>175</v>
+      </c>
+      <c r="B178" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>176</v>
-      </c>
-      <c r="B177" t="s">
+      <c r="C178">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>175</v>
+      </c>
+      <c r="B179" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>176</v>
-      </c>
-      <c r="B178" t="s">
+      <c r="C179">
+        <v>1954</v>
+      </c>
+      <c r="D179">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>175</v>
+      </c>
+      <c r="B180" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>176</v>
-      </c>
-      <c r="B179" t="s">
+      <c r="C180">
+        <v>1952</v>
+      </c>
+      <c r="D180">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>175</v>
+      </c>
+      <c r="B181" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>176</v>
-      </c>
-      <c r="B180" t="s">
+      <c r="C181">
+        <v>1953</v>
+      </c>
+      <c r="D181">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>175</v>
+      </c>
+      <c r="B182" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>176</v>
-      </c>
-      <c r="B181" t="s">
+      <c r="C182">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>175</v>
+      </c>
+      <c r="B183" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>176</v>
-      </c>
-      <c r="B182" t="s">
+      <c r="C183">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>175</v>
+      </c>
+      <c r="B184" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>176</v>
-      </c>
-      <c r="B183" t="s">
+      <c r="C184">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>175</v>
+      </c>
+      <c r="B185" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>176</v>
-      </c>
-      <c r="B184" t="s">
+      <c r="C185">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>175</v>
+      </c>
+      <c r="B186" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>176</v>
-      </c>
-      <c r="B185" t="s">
+      <c r="C186">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>175</v>
+      </c>
+      <c r="B187" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>176</v>
-      </c>
-      <c r="B186" t="s">
+      <c r="C187">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>175</v>
+      </c>
+      <c r="B188" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>176</v>
-      </c>
-      <c r="B187" t="s">
+      <c r="C188">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>175</v>
+      </c>
+      <c r="B189" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>176</v>
-      </c>
-      <c r="B188" t="s">
+      <c r="C189">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>175</v>
+      </c>
+      <c r="B190" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>176</v>
-      </c>
-      <c r="B189" t="s">
+      <c r="C190">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>175</v>
+      </c>
+      <c r="B191" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>176</v>
-      </c>
-      <c r="B190" t="s">
+      <c r="C191">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>175</v>
+      </c>
+      <c r="B192" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>176</v>
-      </c>
-      <c r="B191" t="s">
+      <c r="C192">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>175</v>
+      </c>
+      <c r="B193" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>176</v>
-      </c>
-      <c r="B192" t="s">
+      <c r="C193">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>175</v>
+      </c>
+      <c r="B194" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>176</v>
-      </c>
-      <c r="B193" t="s">
-        <v>200</v>
+      <c r="C194">
+        <v>1966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>